<commit_message>
Updated content fixed admin and certificate errors
</commit_message>
<xml_diff>
--- a/src/data/clean_data_new.xlsx
+++ b/src/data/clean_data_new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\OneDrive\Documents\GitHub\ExperimentEH\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{4E61CB91-9F18-4BFA-A133-1A110597D4E1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8FA322D-2BC6-42A5-983A-33A93CE96DB0}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{4E61CB91-9F18-4BFA-A133-1A110597D4E1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{AEE85215-85AA-44BA-9013-081844EAFFD7}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -112,7 +112,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>admin:</t>
         </r>
@@ -121,7 +121,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 this amount is to be combined with the evaluation sentence. The amount itself is fixed to the startup.</t>
@@ -160,7 +160,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>admin:</t>
         </r>
@@ -169,7 +169,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 This is fixed to the startup. We only randomize the first names.</t>
@@ -401,12 +401,6 @@
     <t>According to the founder’s internal valuation model, the business is worth</t>
   </si>
   <si>
-    <t>Sequoia Capital set a pre-money valuation of the start-up at</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Based on internal benchmarks, the start-up's founder estimates its worth at  </t>
-  </si>
-  <si>
     <t>Founder_firstname_altered</t>
   </si>
   <si>
@@ -483,13 +477,19 @@
   </si>
   <si>
     <t>Thompson</t>
+  </si>
+  <si>
+    <t>Venture capital firm Sequoia set a pre-money valuation of the start-up at</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using internal performance indicators, the founder estimates the start-up's value at  </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -525,19 +525,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -878,7 +865,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="48.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -906,13 +893,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>4</v>
@@ -933,19 +920,19 @@
         <v>8</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E2" s="4">
         <v>2016</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G2" s="4">
         <v>35</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I2" s="4"/>
     </row>
@@ -960,19 +947,19 @@
         <v>11</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E3" s="4">
         <v>2020</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G3" s="4">
         <v>34</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I3" s="4"/>
     </row>
@@ -987,19 +974,19 @@
         <v>14</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E4" s="4">
         <v>2011</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G4" s="4">
         <v>35</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I4" s="4"/>
     </row>
@@ -1014,19 +1001,19 @@
         <v>17</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E5" s="4">
         <v>2018</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G5" s="4">
         <v>35</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I5" s="4"/>
     </row>
@@ -1041,19 +1028,19 @@
         <v>20</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E6" s="4">
         <v>2015</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G6" s="4">
         <v>27</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I6" s="4"/>
     </row>
@@ -1068,19 +1055,19 @@
         <v>23</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E7" s="4">
         <v>2023</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G7" s="4">
         <v>27</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I7" s="4"/>
     </row>
@@ -1165,47 +1152,47 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
@@ -1239,7 +1226,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B129C1FF-A6A4-4674-8988-1354FBDEAAA7}">
   <dimension ref="A1:A18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1278,12 +1267,12 @@
     </row>
     <row r="7" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated instructions, startup data, kept one control photo, updated price and added completion code
</commit_message>
<xml_diff>
--- a/src/data/clean_data_new.xlsx
+++ b/src/data/clean_data_new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\OneDrive\Documents\GitHub\ExperimentEH\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{4E61CB91-9F18-4BFA-A133-1A110597D4E1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{AEE85215-85AA-44BA-9013-081844EAFFD7}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{4E61CB91-9F18-4BFA-A133-1A110597D4E1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A8E44E1-3393-4528-926B-E29B25464045}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -224,6 +224,78 @@
         </r>
       </text>
     </comment>
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{5518EABD-15F5-40A2-A08F-59453999F13D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+increase from 2016</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{36FDC1AB-A888-4698-98A0-2D76AB0AC19F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+increase from original 2011 to match lowest founder age</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E6" authorId="0" shapeId="0" xr:uid="{55DA739B-227A-45C5-8498-7A05946A9644}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+increase from 2015</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -325,52 +397,34 @@
     <t>Biotechnology</t>
   </si>
   <si>
-    <t>Regenary specializes in regenerative medicine, developing a novel biological platform that replaces and regenerates body tissues.</t>
-  </si>
-  <si>
     <t>SkyrOn</t>
   </si>
   <si>
     <t>Consumer Electronics</t>
   </si>
   <si>
-    <t>SkyrOn delivers drone analytics solutions by providing commercial unmanned aerial vehicles tailored for enterprise use.</t>
-  </si>
-  <si>
     <t>Expada</t>
   </si>
   <si>
     <t>Apps</t>
   </si>
   <si>
-    <t>Expada develops a cloud-embedded platform that enables manufacturers and retailers to connect their products to web and smartphone apps.</t>
-  </si>
-  <si>
     <t>TacitFrame</t>
   </si>
   <si>
     <t>Data and Analytics</t>
   </si>
   <si>
-    <t>TacitFrame provides premier brand safety and contextual analytics solutions for digital video content worldwide.</t>
-  </si>
-  <si>
     <t>Aegisline</t>
   </si>
   <si>
     <t>Health Care</t>
   </si>
   <si>
-    <t>Aegisline develops healthcare technology with a special focus on telemedicine innovations.</t>
-  </si>
-  <si>
     <t>Lendr</t>
   </si>
   <si>
     <t>Financial Services</t>
-  </si>
-  <si>
-    <t>Lendr offers a new credit card solution designed to move small dollar loan customers into a more affordable product.</t>
   </si>
   <si>
     <r>
@@ -484,12 +538,30 @@
   <si>
     <t xml:space="preserve">Using internal performance indicators, the founder estimates the start-up's value at  </t>
   </si>
+  <si>
+    <t>The start-up specializes in regenerative medicine, developing a novel biological platform that replaces and regenerates body tissues.</t>
+  </si>
+  <si>
+    <t>The start-up delivers drone analytics solutions by providing commercial unmanned aerial vehicles tailored for enterprise use.</t>
+  </si>
+  <si>
+    <t>The start-up develops a cloud-embedded platform that enables manufacturers and retailers to connect their products to web and smartphone apps.</t>
+  </si>
+  <si>
+    <t>The start-up provides premier brand safety and contextual analytics solutions for digital video content worldwide.</t>
+  </si>
+  <si>
+    <t>The start-up develops healthcare technology with a special focus on telemedicine innovations.</t>
+  </si>
+  <si>
+    <t>The start-up offers a new credit card solution designed to move small dollar loan customers into a more affordable product.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -525,6 +597,19 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -865,7 +950,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="48.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -893,13 +978,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>4</v>
@@ -917,157 +1002,157 @@
         <v>7</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E2" s="4">
-        <v>2016</v>
+        <v>2018</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G2" s="4">
         <v>35</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>10</v>
-      </c>
       <c r="C3" s="4" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E3" s="4">
         <v>2020</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="G3" s="4">
         <v>34</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="4">
+        <v>2016</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="E4" s="4">
-        <v>2011</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="G4" s="4">
         <v>35</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="I4" s="4"/>
     </row>
     <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E5" s="4">
         <v>2018</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="G5" s="4">
         <v>35</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="4">
+        <v>2017</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="E6" s="4">
-        <v>2015</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="G6" s="4">
         <v>27</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="I6" s="4"/>
     </row>
     <row r="7" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E7" s="4">
         <v>2023</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G7" s="4">
         <v>27</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="I7" s="4"/>
     </row>
@@ -1152,47 +1237,47 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
@@ -1226,7 +1311,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B129C1FF-A6A4-4674-8988-1354FBDEAAA7}">
   <dimension ref="A1:A18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -1242,37 +1327,37 @@
     </row>
     <row r="2" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Generated nstartupsets=2000 and nnewscodes=1400 700 each
</commit_message>
<xml_diff>
--- a/src/data/clean_data_new.xlsx
+++ b/src/data/clean_data_new.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\OneDrive\Documents\GitHub\ExperimentEH\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\OneDrive\Documents\GitHub\ExperimentGBTC\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{4E61CB91-9F18-4BFA-A133-1A110597D4E1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A8E44E1-3393-4528-926B-E29B25464045}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{4E61CB91-9F18-4BFA-A133-1A110597D4E1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{6CFE4785-E627-45D2-9166-4D01F4ECCE62}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -176,7 +176,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{B1AB94E2-C7EB-48BC-916B-6A0DD62858AA}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{A3A5AAA5-188C-4CE8-86DE-A7B1E75FD7D8}">
       <text>
         <r>
           <rPr>
@@ -184,7 +184,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t>admin:</t>
         </r>
@@ -193,14 +193,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-fixed pilot 1. randomize pilot.</t>
+Fixed to startup</t>
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{7044A92D-16C1-46AF-A179-2EA8DE0A268B}">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{05C29ADD-766D-438A-9803-B417989A111E}">
       <text>
         <r>
           <rPr>
@@ -208,7 +208,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t>admin:</t>
         </r>
@@ -217,10 +217,10 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-fixed pilot 1</t>
+Fixed to startup</t>
         </r>
       </text>
     </comment>
@@ -950,7 +950,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="48.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>